<commit_message>
fix download excel file
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1247,6 +1247,302 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>TRƯƠNG THÀNH TAM</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>080427</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>10:34</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>B/T</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2024-04-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>TRƯƠNG TƯ XUÂN</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>080262</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>10:34</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2024-04-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>LÊ THANH TUẤN</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>101339</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>10:37</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2024-04-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>LÊ PHƯƠNG</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>070032</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>10:38</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2024-04-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>TRƯƠNG THÀNH TAM</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>080427</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>10:38</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>B/T</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2024-04-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>LÊ THANH TUẤN</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>101339</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>10:39</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2024-04-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>NGUYỄN HOÀNG VIỆT</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>172759</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>10:39</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2024-04-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>BÙI ĐÌNH HỒNG PHÚC</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>193273</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>10:39</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>TEST REQUEST</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>RD</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2024-04-11</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>